<commit_message>
Stap 1 avg cum per maand
</commit_message>
<xml_diff>
--- a/Overzicht_per_maand.xlsx
+++ b/Overzicht_per_maand.xlsx
@@ -28,193 +28,193 @@
     <t>month_yr</t>
   </si>
   <si>
-    <t>Apr-2014</t>
-  </si>
-  <si>
-    <t>Apr-2015</t>
-  </si>
-  <si>
-    <t>Apr-2016</t>
-  </si>
-  <si>
-    <t>Apr-2017</t>
-  </si>
-  <si>
-    <t>Apr-2018</t>
-  </si>
-  <si>
-    <t>Apr-2019</t>
-  </si>
-  <si>
-    <t>Aug-2015</t>
-  </si>
-  <si>
-    <t>Aug-2016</t>
-  </si>
-  <si>
-    <t>Aug-2017</t>
-  </si>
-  <si>
-    <t>Aug-2018</t>
-  </si>
-  <si>
-    <t>Aug-2019</t>
-  </si>
-  <si>
-    <t>Dec-2014</t>
-  </si>
-  <si>
-    <t>Dec-2015</t>
-  </si>
-  <si>
-    <t>Dec-2016</t>
-  </si>
-  <si>
-    <t>Dec-2017</t>
-  </si>
-  <si>
-    <t>Dec-2018</t>
-  </si>
-  <si>
-    <t>Feb-2015</t>
-  </si>
-  <si>
-    <t>Feb-2016</t>
-  </si>
-  <si>
-    <t>Feb-2017</t>
-  </si>
-  <si>
-    <t>Feb-2018</t>
-  </si>
-  <si>
-    <t>Feb-2019</t>
-  </si>
-  <si>
-    <t>Jan-2015</t>
-  </si>
-  <si>
-    <t>Jan-2016</t>
-  </si>
-  <si>
-    <t>Jan-2017</t>
-  </si>
-  <si>
-    <t>Jan-2018</t>
-  </si>
-  <si>
-    <t>Jan-2019</t>
-  </si>
-  <si>
-    <t>Jul-2014</t>
-  </si>
-  <si>
-    <t>Jul-2015</t>
-  </si>
-  <si>
-    <t>Jul-2016</t>
-  </si>
-  <si>
-    <t>Jul-2017</t>
-  </si>
-  <si>
-    <t>Jul-2018</t>
-  </si>
-  <si>
-    <t>Jul-2019</t>
-  </si>
-  <si>
-    <t>Jun-2015</t>
-  </si>
-  <si>
-    <t>Jun-2016</t>
-  </si>
-  <si>
-    <t>Jun-2017</t>
-  </si>
-  <si>
-    <t>Jun-2018</t>
-  </si>
-  <si>
-    <t>Jun-2019</t>
-  </si>
-  <si>
-    <t>Mar-2015</t>
-  </si>
-  <si>
-    <t>Mar-2016</t>
-  </si>
-  <si>
-    <t>Mar-2017</t>
-  </si>
-  <si>
-    <t>Mar-2018</t>
-  </si>
-  <si>
-    <t>Mar-2019</t>
-  </si>
-  <si>
-    <t>May-2015</t>
-  </si>
-  <si>
-    <t>May-2016</t>
-  </si>
-  <si>
-    <t>May-2017</t>
-  </si>
-  <si>
-    <t>May-2018</t>
-  </si>
-  <si>
-    <t>May-2019</t>
-  </si>
-  <si>
-    <t>Nov-2014</t>
-  </si>
-  <si>
-    <t>Nov-2015</t>
-  </si>
-  <si>
-    <t>Nov-2016</t>
-  </si>
-  <si>
-    <t>Nov-2017</t>
-  </si>
-  <si>
-    <t>Nov-2018</t>
-  </si>
-  <si>
-    <t>Oct-2014</t>
-  </si>
-  <si>
-    <t>Oct-2015</t>
-  </si>
-  <si>
-    <t>Oct-2016</t>
-  </si>
-  <si>
-    <t>Oct-2017</t>
-  </si>
-  <si>
-    <t>Oct-2018</t>
-  </si>
-  <si>
-    <t>Sep-2014</t>
-  </si>
-  <si>
-    <t>Sep-2015</t>
-  </si>
-  <si>
-    <t>Sep-2016</t>
-  </si>
-  <si>
-    <t>Sep-2017</t>
-  </si>
-  <si>
-    <t>Sep-2018</t>
-  </si>
-  <si>
-    <t>Sep-2019</t>
+    <t>Apr 2014</t>
+  </si>
+  <si>
+    <t>Apr 2015</t>
+  </si>
+  <si>
+    <t>Apr 2016</t>
+  </si>
+  <si>
+    <t>Apr 2017</t>
+  </si>
+  <si>
+    <t>Apr 2018</t>
+  </si>
+  <si>
+    <t>Apr 2019</t>
+  </si>
+  <si>
+    <t>Aug 2015</t>
+  </si>
+  <si>
+    <t>Aug 2016</t>
+  </si>
+  <si>
+    <t>Aug 2017</t>
+  </si>
+  <si>
+    <t>Aug 2018</t>
+  </si>
+  <si>
+    <t>Aug 2019</t>
+  </si>
+  <si>
+    <t>Dec 2014</t>
+  </si>
+  <si>
+    <t>Dec 2015</t>
+  </si>
+  <si>
+    <t>Dec 2016</t>
+  </si>
+  <si>
+    <t>Dec 2017</t>
+  </si>
+  <si>
+    <t>Dec 2018</t>
+  </si>
+  <si>
+    <t>Feb 2015</t>
+  </si>
+  <si>
+    <t>Feb 2016</t>
+  </si>
+  <si>
+    <t>Feb 2017</t>
+  </si>
+  <si>
+    <t>Feb 2018</t>
+  </si>
+  <si>
+    <t>Feb 2019</t>
+  </si>
+  <si>
+    <t>Jan 2015</t>
+  </si>
+  <si>
+    <t>Jan 2016</t>
+  </si>
+  <si>
+    <t>Jan 2017</t>
+  </si>
+  <si>
+    <t>Jan 2018</t>
+  </si>
+  <si>
+    <t>Jan 2019</t>
+  </si>
+  <si>
+    <t>Jul 2014</t>
+  </si>
+  <si>
+    <t>Jul 2015</t>
+  </si>
+  <si>
+    <t>Jul 2016</t>
+  </si>
+  <si>
+    <t>Jul 2017</t>
+  </si>
+  <si>
+    <t>Jul 2018</t>
+  </si>
+  <si>
+    <t>Jul 2019</t>
+  </si>
+  <si>
+    <t>Jun 2015</t>
+  </si>
+  <si>
+    <t>Jun 2016</t>
+  </si>
+  <si>
+    <t>Jun 2017</t>
+  </si>
+  <si>
+    <t>Jun 2018</t>
+  </si>
+  <si>
+    <t>Jun 2019</t>
+  </si>
+  <si>
+    <t>Mar 2015</t>
+  </si>
+  <si>
+    <t>Mar 2016</t>
+  </si>
+  <si>
+    <t>Mar 2017</t>
+  </si>
+  <si>
+    <t>Mar 2018</t>
+  </si>
+  <si>
+    <t>Mar 2019</t>
+  </si>
+  <si>
+    <t>May 2015</t>
+  </si>
+  <si>
+    <t>May 2016</t>
+  </si>
+  <si>
+    <t>May 2017</t>
+  </si>
+  <si>
+    <t>May 2018</t>
+  </si>
+  <si>
+    <t>May 2019</t>
+  </si>
+  <si>
+    <t>Nov 2014</t>
+  </si>
+  <si>
+    <t>Nov 2015</t>
+  </si>
+  <si>
+    <t>Nov 2016</t>
+  </si>
+  <si>
+    <t>Nov 2017</t>
+  </si>
+  <si>
+    <t>Nov 2018</t>
+  </si>
+  <si>
+    <t>Oct 2014</t>
+  </si>
+  <si>
+    <t>Oct 2015</t>
+  </si>
+  <si>
+    <t>Oct 2016</t>
+  </si>
+  <si>
+    <t>Oct 2017</t>
+  </si>
+  <si>
+    <t>Oct 2018</t>
+  </si>
+  <si>
+    <t>Sep 2014</t>
+  </si>
+  <si>
+    <t>Sep 2015</t>
+  </si>
+  <si>
+    <t>Sep 2016</t>
+  </si>
+  <si>
+    <t>Sep 2017</t>
+  </si>
+  <si>
+    <t>Sep 2018</t>
+  </si>
+  <si>
+    <t>Sep 2019</t>
   </si>
 </sst>
 </file>

</xml_diff>